<commit_message>
add check for unique and not empty. Has error
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>INN</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -415,6 +415,33 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>987654321</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>